<commit_message>
Rearrange the repository, added entry for values of the RQ1
</commit_message>
<xml_diff>
--- a/DataExtraction/Performance.xlsx
+++ b/DataExtraction/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/Projects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDD2375-2B7D-CC45-8356-A43F7C44FD12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFBC04-ABD8-8643-A886-2268C0131546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
+    <workbookView xWindow="4780" yWindow="1340" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
-  <si>
-    <t>Paper</t>
-  </si>
-  <si>
-    <t>Pages</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Rate</t>
   </si>
@@ -223,6 +219,18 @@
   </si>
   <si>
     <t xml:space="preserve">This paper is familiar. </t>
+  </si>
+  <si>
+    <t>Task and Paper</t>
+  </si>
+  <si>
+    <t>Fill up RQ1</t>
+  </si>
+  <si>
+    <t>Pages or Items</t>
+  </si>
+  <si>
+    <t>Work on the values of RQ1</t>
   </si>
 </sst>
 </file>
@@ -616,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF0510-1FDD-3544-BE56-95975250B98E}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,21 +638,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>7</v>
@@ -653,13 +661,13 @@
         <v>21</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D46" si="0">C2/B2</f>
+        <f t="shared" ref="D2:D49" si="0">C2/B2</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
@@ -674,7 +682,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
@@ -689,7 +697,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -704,7 +712,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -719,7 +727,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -734,7 +742,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>12</v>
@@ -749,7 +757,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>17</v>
@@ -762,12 +770,12 @@
         <v>1.6470588235294117</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
@@ -782,7 +790,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>7</v>
@@ -797,7 +805,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
@@ -810,12 +818,12 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>11</v>
@@ -830,7 +838,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>6</v>
@@ -845,7 +853,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>6</v>
@@ -860,7 +868,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
@@ -873,12 +881,12 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>6</v>
@@ -891,12 +899,12 @@
         <v>4.166666666666667</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
@@ -909,12 +917,12 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>6</v>
@@ -927,12 +935,12 @@
         <v>2.6666666666666665</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>4</v>
@@ -947,7 +955,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>4</v>
@@ -962,7 +970,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>5</v>
@@ -975,12 +983,12 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>5</v>
@@ -995,7 +1003,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>6</v>
@@ -1010,7 +1018,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>6</v>
@@ -1023,12 +1031,12 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1">
         <v>6</v>
@@ -1041,12 +1049,12 @@
         <v>2.5</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1">
         <v>6</v>
@@ -1059,12 +1067,12 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
         <v>7</v>
@@ -1077,12 +1085,12 @@
         <v>2.4285714285714284</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1">
         <v>9</v>
@@ -1095,12 +1103,12 @@
         <v>5.1111111111111107</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1">
         <v>9</v>
@@ -1113,12 +1121,12 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1">
         <v>9</v>
@@ -1131,12 +1139,12 @@
         <v>2.8888888888888888</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" s="1">
         <v>10</v>
@@ -1151,7 +1159,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="1">
         <v>12</v>
@@ -1166,7 +1174,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1">
         <v>12</v>
@@ -1179,12 +1187,12 @@
         <v>1.5</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1">
         <v>12</v>
@@ -1199,7 +1207,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1">
         <v>13</v>
@@ -1212,12 +1220,12 @@
         <v>2.0769230769230771</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B40" s="1">
         <v>14</v>
@@ -1230,12 +1238,12 @@
         <v>1.5714285714285714</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1">
         <v>15</v>
@@ -1250,7 +1258,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1">
         <v>16</v>
@@ -1265,7 +1273,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1">
         <v>18</v>
@@ -1278,12 +1286,12 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B44" s="1">
         <v>18</v>
@@ -1298,7 +1306,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1">
         <v>24</v>
@@ -1313,7 +1321,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1">
         <v>21</v>
@@ -1326,7 +1334,33 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="E46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>63</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1">
+        <v>60</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished revamping RQ1, added RQ1 values for new papers, finished drawing RQ1 figures
</commit_message>
<xml_diff>
--- a/DataExtraction/Performance.xlsx
+++ b/DataExtraction/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/Projects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFBC04-ABD8-8643-A886-2268C0131546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1839B2-D587-C645-A19B-8808D6299769}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="1340" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
+    <workbookView xWindow="2820" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Rate</t>
   </si>
@@ -231,6 +229,21 @@
   </si>
   <si>
     <t>Work on the values of RQ1</t>
+  </si>
+  <si>
+    <t>Work on the value of RQ1</t>
+  </si>
+  <si>
+    <t>Update the technical problems, remove "remove trusted third party" and other generic values</t>
+  </si>
+  <si>
+    <t>Update the improvement objectives to add proper new functionality</t>
+  </si>
+  <si>
+    <t>Finish adding values for RQ1</t>
+  </si>
+  <si>
+    <t>Finish drawing new figures for RQ1</t>
   </si>
 </sst>
 </file>
@@ -624,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF0510-1FDD-3544-BE56-95975250B98E}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D49" si="0">C2/B2</f>
+        <f t="shared" ref="D2:D46" si="0">C2/B2</f>
         <v>3</v>
       </c>
     </row>
@@ -1347,10 +1360,6 @@
       <c r="C48" s="1">
         <v>60</v>
       </c>
-      <c r="D48" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -1361,6 +1370,62 @@
       </c>
       <c r="C49" s="1">
         <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <f>60*3+17</f>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revamp values of RQ2.1 and added entries from new papers
</commit_message>
<xml_diff>
--- a/DataExtraction/Performance.xlsx
+++ b/DataExtraction/Performance.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1839B2-D587-C645-A19B-8808D6299769}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2444DBD4-6C5A-7040-A35B-E0392E297A8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Rate</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Finish drawing new figures for RQ1</t>
+  </si>
+  <si>
+    <t>Note and update values of RQ2.1</t>
+  </si>
+  <si>
+    <t>Updates the values of RQ2.1 and add values of new papers</t>
   </si>
 </sst>
 </file>
@@ -637,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF0510-1FDD-3544-BE56-95975250B98E}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:C55"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,6 +1432,28 @@
       </c>
       <c r="C55" s="1">
         <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the performance file
</commit_message>
<xml_diff>
--- a/DataExtraction/Performance.xlsx
+++ b/DataExtraction/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2444DBD4-6C5A-7040-A35B-E0392E297A8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62998D74-2580-D540-AE59-D77E8AF2875A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Rate</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Updates the values of RQ2.1 and add values of new papers</t>
+  </si>
+  <si>
+    <t>Create new figures for RQ2.1</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF0510-1FDD-3544-BE56-95975250B98E}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="C59" sqref="C57:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,6 +1457,17 @@
       </c>
       <c r="C58" s="1">
         <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish updating extraction data
</commit_message>
<xml_diff>
--- a/DataExtraction/Performance.xlsx
+++ b/DataExtraction/Performance.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/Projects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62998D74-2580-D540-AE59-D77E8AF2875A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2CB137-346D-CD46-8CDD-1C242F4BBAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
+    <workbookView xWindow="2800" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{EEE11444-ED42-A84B-90DD-242126287D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Rate</t>
   </si>
@@ -253,6 +255,33 @@
   </si>
   <si>
     <t>Create new figures for RQ2.1</t>
+  </si>
+  <si>
+    <t>New values of RQ2.1 on deployment, add new values</t>
+  </si>
+  <si>
+    <t>Revampe values for RQ2.2 on on-chain data</t>
+  </si>
+  <si>
+    <t>Revamp and add values to RQ2.2</t>
+  </si>
+  <si>
+    <t>Make figures for RQ2.2</t>
+  </si>
+  <si>
+    <t>Revamp values for RQ2.2 on on-chain logic</t>
+  </si>
+  <si>
+    <t>Add values of new papers to RQ2.2 on on-chain logic</t>
+  </si>
+  <si>
+    <t>Draw new figures for RQ2.2 on on-chain logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update and add values for RQ2.3 </t>
+  </si>
+  <si>
+    <t>Update values for RQ3, add new values, draw figures</t>
   </si>
 </sst>
 </file>
@@ -646,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EF0510-1FDD-3544-BE56-95975250B98E}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C59" sqref="C57:C59"/>
+      <selection activeCell="C69" sqref="C61:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1468,6 +1497,105 @@
       </c>
       <c r="C59" s="1">
         <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>